<commit_message>
Product Backlog Final 9.12
</commit_message>
<xml_diff>
--- a/S24 Product Backlog - updated 08112024 - TIIMI1.xlsx
+++ b/S24 Product Backlog - updated 08112024 - TIIMI1.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h01340\OneDrive - Haaga-Helia Oy Ab\1-Ohjelmistoprojekti1\s24\tiimi1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia.sharepoint.com/teams/Ohjelmistoprojekti1-tiimi341/Jaetut asiakirjat/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15302343-EEEA-4CC8-B36E-1D0597E28E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F36D0A2-1D5C-4EC6-935F-60533093723C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C479CED9-8A31-459B-9A34-852820542566}"/>
+    <workbookView xWindow="1080" yWindow="500" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="2" xr2:uid="{C479CED9-8A31-459B-9A34-852820542566}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="pilot-velocity" sheetId="2" r:id="rId2"/>
-    <sheet name="burndown" sheetId="3" r:id="rId3"/>
+    <sheet name="Tiedot1" sheetId="4" r:id="rId2"/>
+    <sheet name="pilot-velocity" sheetId="2" r:id="rId3"/>
+    <sheet name="burndown" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'pilot-velocity'!$A$1:$B$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'pilot-velocity'!$A$1:$B$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$A$1:$J$59</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="1142" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -234,7 +235,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -243,12 +244,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Vaatimuksen uniikki numero, käytä juoksevaa numerointia</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vaatimuksen uniikki numero, käytä juoksevaa numerointia</t>
         </r>
       </text>
     </comment>
@@ -257,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="260">
   <si>
     <t>Req Nbr</t>
   </si>
@@ -284,6 +294,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Sprint #</t>
   </si>
   <si>
     <t>a) Kehitysympäristö</t>
@@ -856,6 +869,9 @@
     <t xml:space="preserve">Koodi testattu toimivaksi (testit joko manuaalisia tai junit-testejä) &amp; löytyy versionhallinnasta. </t>
   </si>
   <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">…nähdä, kuinka paljon tuotteita on kaupassa saatavilla. </t>
   </si>
   <si>
@@ -1028,10 +1044,50 @@
     <t xml:space="preserve">Tyyppi-tiedot ovat saatavilla ja ns. fixed. </t>
   </si>
   <si>
+    <t>..spring boot sovelluksen käyttöliittymä on "hyvän näköinen" ja helppokäyttöinen</t>
+  </si>
+  <si>
+    <t>Käyttäjäystävällisen ja laadukkaan näköinen sovellus luo luotettavuutta koko yritystä kohden. </t>
+  </si>
+  <si>
+    <t>Tiimi päättää itse, minkälainen tulee olemaan sovelluksen ulkoasu. </t>
+  </si>
+  <si>
+    <t>Tiimin jäsenet ovat tyytyväisiä käyttöliittymän ulkoasuun. </t>
+  </si>
+  <si>
+    <t>e) Sovellus / Front end</t>
+  </si>
+  <si>
+    <t>loppukäyttäjän sovellus on "hyvän näköinen" ja helppokäyttöinen</t>
+  </si>
+  <si>
+    <t>kaupan asiakas voi rekisteröityä kaupan asiakkaaksi. Minimitiedot ovat etu-, sukunimi ja email osoite</t>
+  </si>
+  <si>
+    <t>ks muut tiedot vaatimuksesta 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Loppuasiakas voi varata kaupan tuotteista jonkin ja hakea sen sitten kivijalkaliikkeestä. </t>
+  </si>
+  <si>
+    <t>Kapuan asiakas pystyy varaamaan tuotteita, jotta tuote olisi saatavilla kun menee kauppaan. </t>
+  </si>
+  <si>
+    <t>Sivu, jossa käyttäjä voi varata tuotteen</t>
+  </si>
+  <si>
+    <t>Tiedot: Summa  / Req Nbr - Sprint#: 0 Sprint</t>
+  </si>
+  <si>
     <t>Sprint#</t>
   </si>
   <si>
-    <t>not done</t>
+    <t>0 Sprint</t>
   </si>
   <si>
     <t xml:space="preserve">Velocity mittaa, kuinka paljon tiimi saa valmiiksi (esimerkiksi tarinapisteinä tai tehtävinä) yhdessä sprintissä. </t>
@@ -1040,47 +1096,41 @@
     <t>Tässä tapauksessa lasketaan valmiiksi saatettujen tehtävien määrä sprinttikohtaisesti.</t>
   </si>
   <si>
-    <t>Row Labels</t>
+    <t>Riviotsikot</t>
+  </si>
+  <si>
+    <t>Määrä  / Req Nbr</t>
+  </si>
+  <si>
+    <t>1 Sprint</t>
+  </si>
+  <si>
+    <t>Keskimääräinen velocity eli tiimin kehitysnopeus</t>
+  </si>
+  <si>
+    <t>2 Sprint</t>
+  </si>
+  <si>
+    <t>3 Sprint</t>
+  </si>
+  <si>
+    <t>4 Sprint</t>
+  </si>
+  <si>
+    <t>Kaikki yhteensä</t>
   </si>
   <si>
     <t>Count of Req Nbr</t>
   </si>
   <si>
-    <t>Keskimääräinen velocity eli tiimin kehitysnopeus</t>
-  </si>
-  <si>
-    <t>(blank)</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>0 Sprint</t>
-  </si>
-  <si>
-    <t>1 Sprint</t>
-  </si>
-  <si>
-    <t>2 Sprint</t>
-  </si>
-  <si>
-    <t>3 Sprint</t>
-  </si>
-  <si>
-    <t>Lopusta  puuttuu uusimmat</t>
-  </si>
-  <si>
     <t>Cumulative</t>
-  </si>
-  <si>
-    <t>Sprint #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1144,8 +1194,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1167,6 +1267,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,20 +1302,24 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1247,10 +1357,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1262,9 +1368,39 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1282,7 +1418,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fi-FI"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1344,7 +1480,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fi-FI"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1596,7 +1732,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fi-FI"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="511658879"/>
@@ -1656,7 +1792,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fi-FI"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="511653599"/>
@@ -1698,7 +1834,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fi-FI"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1735,7 +1871,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fi-FI"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2312,8 +2448,8 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38837</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>467462</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>152458</xdr:rowOff>
     </xdr:to>
@@ -2393,22 +2529,24 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Pellikka Minna" refreshedDate="45628.34130659722" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="61" xr:uid="{F656E4C1-8E04-46D4-8641-ED8109B331C5}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Excel Services" refreshedDate="45635.000413773145" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="60" xr:uid="{6C178BAA-1522-B842-BD80-8D611C9FB060}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:B1048576" sheet="pilot-velocity"/>
+    <worksheetSource ref="A1:B61" sheet="pilot-velocity"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="Req Nbr" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="60"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="60"/>
     </cacheField>
     <cacheField name="Sprint#" numFmtId="0">
-      <sharedItems containsBlank="1" count="6">
+      <sharedItems count="8">
         <s v="0 Sprint"/>
         <s v="1 Sprint"/>
         <s v="2 Sprint"/>
         <s v="3 Sprint"/>
-        <s v="not done"/>
-        <m/>
+        <s v="4 Sprint"/>
+        <s v="4 Sprint " u="1"/>
+        <s v="2 Sprint " u="1"/>
+        <s v="3 Sprint " u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -2421,7 +2559,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="61">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
   <r>
     <n v="1"/>
     <x v="0"/>
@@ -2520,7 +2658,7 @@
   </r>
   <r>
     <n v="25"/>
-    <x v="4"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="26"/>
@@ -2580,7 +2718,7 @@
   </r>
   <r>
     <n v="40"/>
-    <x v="4"/>
+    <x v="2"/>
   </r>
   <r>
     <n v="41"/>
@@ -2604,11 +2742,11 @@
   </r>
   <r>
     <n v="46"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="47"/>
-    <x v="4"/>
+    <x v="2"/>
   </r>
   <r>
     <n v="48"/>
@@ -2616,19 +2754,19 @@
   </r>
   <r>
     <n v="49"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="50"/>
-    <x v="4"/>
+    <x v="2"/>
   </r>
   <r>
     <n v="51"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="52"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="53"/>
@@ -2640,11 +2778,11 @@
   </r>
   <r>
     <n v="55"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="56"/>
-    <x v="4"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="57"/>
@@ -2662,26 +2800,24 @@
     <n v="60"/>
     <x v="4"/>
   </r>
-  <r>
-    <m/>
-    <x v="5"/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AEE707F9-533D-44E2-9033-FEE09F36422C}" name="PivotTable7" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D4:E11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9FAD1F43-8DCF-F844-B99A-7EC0A727E724}" name="Pivot-taulukko3" cacheId="1142" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Arvot" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D4:E10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="7">
+      <items count="9">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="6"/>
         <item x="3"/>
+        <item m="1" x="7"/>
         <item x="4"/>
-        <item x="5"/>
+        <item m="1" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2689,7 +2825,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -2700,13 +2836,10 @@
       <x v="2"/>
     </i>
     <i>
-      <x v="3"/>
-    </i>
-    <i>
       <x v="4"/>
     </i>
     <i>
-      <x v="5"/>
+      <x v="6"/>
     </i>
     <i t="grand">
       <x/>
@@ -2716,7 +2849,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of Req Nbr" fld="0" subtotal="count" baseField="1" baseItem="0"/>
+    <dataField name="Määrä  / Req Nbr" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2730,10 +2863,24 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F395FA99-70BE-484E-AAF0-77F3B761498F}" name="Taulukko1" displayName="Taulukko1" ref="A3:B10" totalsRowShown="0">
+  <autoFilter ref="A3:B10" xr:uid="{F395FA99-70BE-484E-AAF0-77F3B761498F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B10">
+    <sortCondition ref="A3:A10"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{821AE20D-24B1-457A-933A-20F452538AA7}" name="Req Nbr"/>
+    <tableColumn id="2" xr3:uid="{A52DA02D-D604-441B-8D03-2FF3996FAD86}" name="Sprint#"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2771,7 +2918,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2877,7 +3024,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3019,7 +3166,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3027,27 +3174,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A41D4B-E510-47CE-BAC3-3E487078559C}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" customWidth="1"/>
-    <col min="5" max="5" width="32.1796875" customWidth="1"/>
-    <col min="6" max="6" width="34.7265625" customWidth="1"/>
-    <col min="7" max="7" width="28.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="4"/>
-    <col min="10" max="10" width="28.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+    <col min="10" max="10" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="33.950000000000003">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3076,1766 +3223,1925 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="66" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="68.45" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" ht="74.099999999999994" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="92.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="92.1" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="117" customHeight="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="117" customHeight="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="71.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="71.099999999999994" customHeight="1">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:10" ht="78.75" customHeight="1">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="62.45" customHeight="1">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:10" ht="84.6" customHeight="1">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="62.45" customHeight="1">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="76.5" customHeight="1">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="63.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="63.6" customHeight="1">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="90" customHeight="1">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="109.5" customHeight="1">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="156" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="156" customHeight="1">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="130.5" customHeight="1">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="78.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:10" ht="78.599999999999994" customHeight="1">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="93" customHeight="1">
       <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="84.75" customHeight="1">
       <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="98" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="90">
       <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="93" customHeight="1">
       <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="134.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:10" ht="134.25" customHeight="1">
       <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="70" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="60">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="70" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="75">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="105.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="105.6" customHeight="1">
       <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="74.099999999999994" customHeight="1">
       <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="106.5" customHeight="1">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="66" customHeight="1">
       <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="H29" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="76.5" customHeight="1">
       <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="62.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="62.1" customHeight="1">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="I31" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="71.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="71.099999999999994" customHeight="1">
       <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="I32" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="74.099999999999994" customHeight="1">
       <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="79.5" customHeight="1">
       <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="105" customHeight="1">
       <c r="A35" s="7">
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="137.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="137.44999999999999" customHeight="1">
       <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="95.45" customHeight="1">
       <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="72.95" customHeight="1">
       <c r="A38" s="7">
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="86.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="86.45" customHeight="1">
       <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="186" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="186" customHeight="1">
       <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I40" s="2"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="1:10" ht="109.4" customHeight="1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="109.35" customHeight="1">
       <c r="A41" s="7">
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="H41" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="84" customHeight="1">
       <c r="A42" s="7">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="56" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="60">
       <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="71.45" customHeight="1">
       <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I44" s="2"/>
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="1:10" ht="56" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="60">
       <c r="A45" s="7">
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F45" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="H45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I45" s="2"/>
-      <c r="J45" s="3"/>
-    </row>
-    <row r="46" spans="1:10" ht="56" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="60">
       <c r="A46" s="7">
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I46" s="2"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="1:10" ht="70" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="60">
       <c r="A47" s="7">
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="1:10" ht="95.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="95.1" customHeight="1">
       <c r="A48" s="7">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I48" s="2"/>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="1:10" ht="167.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="167.1" customHeight="1">
       <c r="A49" s="7">
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I49" s="2"/>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="1:10" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="59.45" customHeight="1">
       <c r="A50" s="7">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I50" s="2"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="1:10" ht="98" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="90">
       <c r="A51" s="7">
         <v>50</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="H51" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="1:10" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="118.5" customHeight="1">
       <c r="A52" s="7">
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I52" s="2"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="1:10" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="118.5" customHeight="1">
       <c r="A53" s="7">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I53" s="2"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="1:10" ht="56" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="60">
       <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I54" s="2"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="55" spans="1:10" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="103.5" customHeight="1">
       <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I55" s="2"/>
-      <c r="J55" s="3"/>
-    </row>
-    <row r="56" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="60" customHeight="1">
       <c r="A56" s="7">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>223</v>
-      </c>
       <c r="G56" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I56" s="2"/>
-      <c r="J56" s="3"/>
-    </row>
-    <row r="57" spans="1:10" ht="70" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="60">
       <c r="A57" s="7">
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I57" s="2"/>
-      <c r="J57" s="3"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A58" s="7">
+        <v>16</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="68.099999999999994">
+      <c r="A58" s="20">
         <v>57</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A59" s="7">
+      <c r="B58" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="H58" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="51">
+      <c r="A59" s="20">
         <v>58</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="3"/>
-    </row>
-    <row r="60" spans="1:10" ht="28" x14ac:dyDescent="0.35">
-      <c r="B60" s="16" t="s">
+      <c r="B59" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="H59" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="84.95">
+      <c r="A60" s="20">
+        <v>59</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="68.099999999999994">
+      <c r="A61" s="20">
+        <v>60</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="F61" s="20" t="s">
         <v>244</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="H61" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4853,29 +5159,123 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D3ECFA-1D55-48ED-AE67-066D255E0A3D}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748C6CA1-44AE-4EB4-9F3D-97E840A65A1B}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="26.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" style="8"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="27"/>
+    <col min="2" max="2" width="12.140625" style="31"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>231</v>
+      <c r="B1" s="28" t="s">
+        <v>246</v>
       </c>
       <c r="D1" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -4885,15 +5285,15 @@
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+    <row r="2" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>240</v>
+      <c r="B2" s="29" t="s">
+        <v>247</v>
       </c>
       <c r="D2" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -4903,12 +5303,12 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+    <row r="3" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>240</v>
+      <c r="B3" s="29" t="s">
+        <v>247</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
@@ -4918,560 +5318,546 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+    <row r="4" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A4" s="25">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>235</v>
+      <c r="B4" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>250</v>
       </c>
       <c r="E4" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+    <row r="5" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A5" s="25">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>240</v>
+      <c r="B5" s="29" t="s">
+        <v>247</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+    <row r="6" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A6" s="25">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>240</v>
+      <c r="B6" s="29" t="s">
+        <v>247</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="E6">
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>240</v>
+      <c r="B7" s="29" t="s">
+        <v>247</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="E7">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G7" s="13">
         <f>SUM(E5:E8)/4</f>
-        <v>9.75</v>
+        <v>12.25</v>
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
+    <row r="8" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>241</v>
+      <c r="B8" s="29" t="s">
+        <v>252</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
+    <row r="9" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>241</v>
+      <c r="B9" s="29" t="s">
+        <v>252</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="E9">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
+    <row r="10" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>241</v>
+      <c r="B10" s="29" t="s">
+        <v>252</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>238</v>
+        <v>257</v>
+      </c>
+      <c r="E10">
+        <v>60</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7">
+    <row r="11" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="E11">
-        <v>60</v>
+      <c r="B11" s="29" t="s">
+        <v>252</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
+    <row r="12" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>241</v>
+      <c r="B12" s="29" t="s">
+        <v>252</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7">
+    <row r="13" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>241</v>
+      <c r="B13" s="29" t="s">
+        <v>252</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7">
+    <row r="14" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7">
+      <c r="B14" s="29" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7">
+      <c r="B15" s="29" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="26.25" customHeight="1">
+      <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7">
+      <c r="B16" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7">
+      <c r="B17" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7">
+      <c r="B18" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="7">
+      <c r="B19" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="I19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="7">
+      <c r="B20" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7">
+      <c r="B21" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
+      <c r="B22" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
+      <c r="B23" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="7">
+      <c r="B24" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7">
+      <c r="B25" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="7">
+      <c r="B26" s="29" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="7">
+      <c r="B27" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="7">
+      <c r="B28" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A29" s="26">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="7">
+      <c r="B29" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A30" s="26">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="7">
+      <c r="B30" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="7">
+      <c r="B31" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="7">
+      <c r="B32" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A33" s="26">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="7">
+      <c r="B33" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A34" s="26">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="7">
+      <c r="B34" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A35" s="26">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="7">
+      <c r="B35" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A36" s="26">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="7">
+      <c r="B36" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A37" s="26">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="7">
+      <c r="B37" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A38" s="26">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="7">
+      <c r="B38" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A39" s="26">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="7">
+      <c r="B39" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A40" s="26">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="7">
+      <c r="B40" s="29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A41" s="26">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="7">
+      <c r="B41" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A42" s="26">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="7">
+      <c r="B42" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A43" s="26">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="7">
+      <c r="B43" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A44" s="26">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="7">
+      <c r="B44" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A45" s="26">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="7">
+      <c r="B45" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A46" s="26">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="7">
+      <c r="B46" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A47" s="26">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="7">
+      <c r="B47" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A48" s="26">
         <v>47</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="7">
+      <c r="B48" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A49" s="26">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="7">
+      <c r="B49" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A50" s="26">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="7">
+      <c r="B50" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A51" s="26">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="7">
+      <c r="B51" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A52" s="26">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="7">
+      <c r="B52" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A53" s="26">
         <v>52</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="7">
+      <c r="B53" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A54" s="26">
         <v>53</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="7">
+      <c r="B54" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A55" s="26">
         <v>54</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="7">
+      <c r="B55" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A56" s="26">
         <v>55</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="7">
+      <c r="B56" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A57" s="26">
         <v>56</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="7">
+      <c r="B57" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A58" s="26">
         <v>57</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="7">
+      <c r="B58" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A59" s="26">
         <v>58</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="7">
+      <c r="B59" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A60" s="26">
         <v>59</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="7">
+      <c r="B60" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A61" s="26">
         <v>60</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>232</v>
+      <c r="B61" s="30" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -5486,84 +5872,84 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C851B51D-AEE5-48CC-8949-660B6EAA1CB7}">
   <dimension ref="B3:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="C4" s="19">
+    <row r="3" spans="2:4">
+      <c r="B3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="17">
         <v>6</v>
       </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" s="19">
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="17">
         <v>8</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="17">
         <f>C4+C5</f>
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="C6" s="19">
+    <row r="6" spans="2:4">
+      <c r="B6" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="17">
         <v>18</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <f>D5+C6</f>
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="C7" s="19">
+    <row r="7" spans="2:4">
+      <c r="B7" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="17">
         <v>7</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="18">
         <f t="shared" ref="D7" si="0">D6+C7</f>
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="C8" s="21">
+    <row r="8" spans="2:4">
+      <c r="B8" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8" s="19">
         <v>21</v>
       </c>
-      <c r="D8" s="21"/>
+      <c r="D8" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5572,42 +5958,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5041c815-b662-4e97-91f9-dfea5c801e6c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000F31C13F2B02C42804791B7D176580F" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b758590bad793664214290192af8eea1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5041c815-b662-4e97-91f9-dfea5c801e6c" xmlns:ns4="6f4f8b50-ea0e-40fb-af4c-f58df4ea5ac5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37d8109bda380f817570ff6b57111f4d" ns3:_="" ns4:_="">
-    <xsd:import namespace="5041c815-b662-4e97-91f9-dfea5c801e6c"/>
-    <xsd:import namespace="6f4f8b50-ea0e-40fb-af4c-f58df4ea5ac5"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x01010061FA388B24C5844A87282C76D8503176" ma:contentTypeVersion="4" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="3cbd16230a07cb6e49d443617b2c6b1a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="24f9f1a4-8b2e-4dc6-a8c3-ac769f41722c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87d31b248dbbb9badc47fdaf789e4726" ns2:_="">
+    <xsd:import namespace="24f9f1a4-8b2e-4dc6-a8c3-ac769f41722c"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns3:_activity" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5615,7 +5978,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5041c815-b662-4e97-91f9-dfea5c801e6c" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="24f9f1a4-8b2e-4dc6-a8c3-ac769f41722c" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -5628,106 +5991,12 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="16" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="19" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="20" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="_activity" ma:index="23" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSystemTags" ma:index="25" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6f4f8b50-ea0e-40fb-af4c-f58df4ea5ac5" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -5742,8 +6011,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Sisältölaji"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Otsikko"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -5832,7 +6101,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5841,39 +6110,20 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0269E476-3EF6-4749-ADF3-0D5C450A2E68}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5041c815-b662-4e97-91f9-dfea5c801e6c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDA8B8D6-5248-48CF-A60F-3FE4ADD0934D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D0DAEF-B02C-4FAE-8C8C-9001DE1D1DA5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5041c815-b662-4e97-91f9-dfea5c801e6c"/>
-    <ds:schemaRef ds:uri="6f4f8b50-ea0e-40fb-af4c-f58df4ea5ac5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEE8F6A6-0841-43B9-BEE5-4DB5A1480306}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEE8F6A6-0841-43B9-BEE5-4DB5A1480306}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0269E476-3EF6-4749-ADF3-0D5C450A2E68}"/>
 </file>
</xml_diff>